<commit_message>
Dictionary reached 18 words
</commit_message>
<xml_diff>
--- a/KanjiDictionary.xlsx
+++ b/KanjiDictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\PyCharm Projects\pythonProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\PyCharm Projects\JapaneseExerciser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
   <si>
     <t>Kanji</t>
   </si>
@@ -68,14 +68,215 @@
     <t>Ue</t>
   </si>
   <si>
-    <t>Onyomi</t>
+    <t>一</t>
+  </si>
+  <si>
+    <t>いち</t>
+  </si>
+  <si>
+    <t>Ichi</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Onyomi - Kunyomi</t>
+  </si>
+  <si>
+    <t>三</t>
+  </si>
+  <si>
+    <t>一, 二</t>
+  </si>
+  <si>
+    <t>さん</t>
+  </si>
+  <si>
+    <t>San</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>才</t>
+  </si>
+  <si>
+    <t>一, 亅, 丿</t>
+  </si>
+  <si>
+    <t>さい</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>Genius</t>
+  </si>
+  <si>
+    <t>大</t>
+  </si>
+  <si>
+    <t>おお</t>
+  </si>
+  <si>
+    <t>Oo</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>八</t>
+  </si>
+  <si>
+    <t>ハ</t>
+  </si>
+  <si>
+    <t>はち</t>
+  </si>
+  <si>
+    <t>Hachi</t>
+  </si>
+  <si>
+    <t>Eight</t>
+  </si>
+  <si>
+    <t>入</t>
+  </si>
+  <si>
+    <t>Nyu</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>にゅう*</t>
+  </si>
+  <si>
+    <t>山</t>
+  </si>
+  <si>
+    <t>やま</t>
+  </si>
+  <si>
+    <t>Yama</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>口</t>
+  </si>
+  <si>
+    <t>くち</t>
+  </si>
+  <si>
+    <t>Kuchi</t>
+  </si>
+  <si>
+    <t>Mouth</t>
+  </si>
+  <si>
+    <t>九</t>
+  </si>
+  <si>
+    <t>きゅう</t>
+  </si>
+  <si>
+    <t>Kyu</t>
+  </si>
+  <si>
+    <t>Nine</t>
+  </si>
+  <si>
+    <t>人</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Hito</t>
+  </si>
+  <si>
+    <t>ひと*</t>
+  </si>
+  <si>
+    <t>力</t>
+  </si>
+  <si>
+    <t>ちから</t>
+  </si>
+  <si>
+    <t>Chikara</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>川</t>
+  </si>
+  <si>
+    <t>かわ</t>
+  </si>
+  <si>
+    <t>Kawa</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>七</t>
+  </si>
+  <si>
+    <t>なな</t>
+  </si>
+  <si>
+    <t>Nana</t>
+  </si>
+  <si>
+    <t>Seven</t>
+  </si>
+  <si>
+    <t>十</t>
+  </si>
+  <si>
+    <t>じゅう</t>
+  </si>
+  <si>
+    <t>Ju</t>
+  </si>
+  <si>
+    <t>Ten</t>
+  </si>
+  <si>
+    <t>二</t>
+  </si>
+  <si>
+    <t>に</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>女</t>
+  </si>
+  <si>
+    <t>おんな</t>
+  </si>
+  <si>
+    <t>Onna</t>
+  </si>
+  <si>
+    <t>Woman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +293,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Default_SC"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
       <name val="Default_SC"/>
       <family val="1"/>
     </font>
@@ -116,10 +323,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +611,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -467,116 +675,276 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>

</xml_diff>